<commit_message>
Update notification student, notification lecturer and notification model
</commit_message>
<xml_diff>
--- a/public/uploads/myTopicDemo.xlsx
+++ b/public/uploads/myTopicDemo.xlsx
@@ -1,38 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnTotNghiep\manage-graduation-thesis-iuh-be\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vscode\manage-graduation-thesis-iuh-be\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0C4994-348C-4B30-84F5-10DB608E4592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="4836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="4836" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Đè tài TN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tri Pham Quang</author>
   </authors>
   <commentList>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Họ tên giảng viên</t>
   </si>
@@ -69,16 +62,7 @@
     <t>Tên đề tài</t>
   </si>
   <si>
-    <t>MỤC TIÊU ĐỀ TÀI</t>
-  </si>
-  <si>
-    <t>DỰ KIẾN SẢN PHẨM NGHIÊN CỨU CỦA ĐỀ TÀI VÀ KHẢ NĂNG ỨNG DỤNG</t>
-  </si>
-  <si>
     <t>Mô tả</t>
-  </si>
-  <si>
-    <t>Yêu cầu đầu ra (Output Standards)</t>
   </si>
   <si>
     <t>- Tìm hiểu cách thức lập trình với WPF. 
@@ -126,9 +110,6 @@
     <t>Mã đề tài</t>
   </si>
   <si>
-    <t>Ứng dụng quản lý khóa luận tốt nghiệp</t>
-  </si>
-  <si>
     <t>Sử dụng để quản lý khóa luận cho toàn khoa</t>
   </si>
   <si>
@@ -137,11 +118,26 @@
   <si>
     <t>01220022</t>
   </si>
+  <si>
+    <t>Website giới thiệu sách mới</t>
+  </si>
+  <si>
+    <t>Website giới thiệu phim mới</t>
+  </si>
+  <si>
+    <t>Mục tiêu đề tài</t>
+  </si>
+  <si>
+    <t>Dự kiến sản phẩm nghiên cứu của đề tài và khả năng ứng dụng</t>
+  </si>
+  <si>
+    <t>Yêu cầu đầu ra</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +311,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -626,13 +622,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA986"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -652,10 +648,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>
@@ -664,19 +660,19 @@
         <v>1</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" s="17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -702,28 +698,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -744,16 +740,34 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+    <row r="3" spans="1:27" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>

</xml_diff>